<commit_message>
test and implement reading gradient fill
</commit_message>
<xml_diff>
--- a/tests/data/reader/formatting.xlsx
+++ b/tests/data/reader/formatting.xlsx
@@ -1,21 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
   <workbookPr date1904="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/Downloads/xlnt/tests/data/reader/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="15960" windowHeight="17460"/>
   </bookViews>
   <sheets>
-    <sheet name="first" sheetId="1" r:id="rId4"/>
-    <sheet name="second" sheetId="2" r:id="rId5"/>
-    <sheet name="third" sheetId="3" r:id="rId6"/>
-    <sheet name="fourth" sheetId="4" r:id="rId7"/>
+    <sheet name="first" sheetId="1" r:id="rId1"/>
+    <sheet name="second" sheetId="2" r:id="rId2"/>
+    <sheet name="third" sheetId="3" r:id="rId3"/>
+    <sheet name="fourth" sheetId="4" r:id="rId4"/>
   </sheets>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>Table 1</t>
   </si>
@@ -133,24 +145,23 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="14">
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="59" formatCode="0.0"/>
-    <numFmt numFmtId="60" formatCode="0.000"/>
-    <numFmt numFmtId="61" formatCode="0.000000000"/>
-    <numFmt numFmtId="62" formatCode="0E+00"/>
-    <numFmt numFmtId="63" formatCode="&quot;$&quot;0.00"/>
-    <numFmt numFmtId="64" formatCode="mmmm d, yyyy"/>
-    <numFmt numFmtId="65" formatCode="[h]&quot;h&quot; m&quot;m&quot; s&quot;s&quot;"/>
-    <numFmt numFmtId="66" formatCode="[$EUR]0.00"/>
-    <numFmt numFmtId="67" formatCode="[$KRW]0.00"/>
-    <numFmt numFmtId="68" formatCode="0,00000000"/>
-    <numFmt numFmtId="69" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="70" formatCode="&quot;$&quot;0.000"/>
-    <numFmt numFmtId="71" formatCode="&quot; &quot;&quot;$&quot;* #,##0.00&quot; &quot;;&quot; &quot;&quot;$&quot;* (#,##0.00&quot;) &quot;;&quot; &quot;&quot;$&quot;* &quot;-&quot;??"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="13">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000000000"/>
+    <numFmt numFmtId="167" formatCode="0E+00"/>
+    <numFmt numFmtId="168" formatCode="&quot;$&quot;0.00"/>
+    <numFmt numFmtId="169" formatCode="mmmm\ d\,\ yyyy"/>
+    <numFmt numFmtId="170" formatCode="[h]&quot;h&quot;\ m&quot;m&quot;\ s&quot;s&quot;"/>
+    <numFmt numFmtId="171" formatCode="[$EUR]0.00"/>
+    <numFmt numFmtId="172" formatCode="[$KRW]0.00"/>
+    <numFmt numFmtId="173" formatCode="000,000,000"/>
+    <numFmt numFmtId="174" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="175" formatCode="&quot;$&quot;0.000"/>
+    <numFmt numFmtId="176" formatCode="&quot; &quot;&quot;$&quot;* #,##0.00&quot; &quot;;&quot; &quot;&quot;$&quot;* \(#,##0.00&quot;) &quot;;&quot; &quot;&quot;$&quot;* &quot;-&quot;??"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -167,12 +178,7 @@
       <name val="Verdana"/>
     </font>
     <font>
-      <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Verdana"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="11"/>
       <name val="Helvetica"/>
@@ -193,25 +199,25 @@
       <name val="Cambria"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
     </font>
     <font>
-      <i val="1"/>
+      <i/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
     </font>
     <font>
-      <strike val="1"/>
+      <strike/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
@@ -222,25 +228,25 @@
       <name val="Cambria"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="21"/>
       <name val="Helvetica"/>
     </font>
     <font>
-      <i val="1"/>
+      <i/>
       <sz val="18"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="8"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -278,10 +284,14 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="8"/>
-        <bgColor auto="1"/>
-      </patternFill>
+      <gradientFill>
+        <stop position="0">
+          <color rgb="FFFF0000"/>
+        </stop>
+        <stop position="1">
+          <color rgb="FF0000FF"/>
+        </stop>
+      </gradientFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -294,6 +304,16 @@
         <fgColor indexed="23"/>
         <bgColor auto="1"/>
       </patternFill>
+    </fill>
+    <fill>
+      <gradientFill type="linear">
+        <stop position="0">
+          <color rgb="FFFF0000"/>
+        </stop>
+        <stop position="1">
+          <color rgb="FF0000FF"/>
+        </stop>
+      </gradientFill>
     </fill>
   </fills>
   <borders count="22">
@@ -589,222 +609,225 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="71">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="59" fontId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="60" fontId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="61" fontId="5" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="62" fontId="4" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="63" fontId="4" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="64" fontId="4" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="65" fontId="4" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="18" fontId="4" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="66" fontId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="67" fontId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="68" fontId="5" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="69" fontId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="70" fontId="5" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="71" fontId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+  <cellXfs count="72">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="18" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="173" fontId="4" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="174" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="175" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="8" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="9" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="9" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -814,7 +837,7 @@
   <dxfs count="1">
     <dxf>
       <font>
-        <color rgb="ff000000"/>
+        <color rgb="FF000000"/>
       </font>
       <fill>
         <patternFill patternType="solid">
@@ -824,40 +847,88 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffa9a9a9"/>
-      <rgbColor rgb="fffefffe"/>
-      <rgbColor rgb="ff578625"/>
-      <rgbColor rgb="ff7f7f7f"/>
-      <rgbColor rgb="ffeeeeee"/>
-      <rgbColor rgb="ff9d44b8"/>
-      <rgbColor rgb="ffffa93a"/>
-      <rgbColor rgb="ff63b2de"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FFA9A9A9"/>
+      <rgbColor rgb="FFFEFFFE"/>
+      <rgbColor rgb="FF578625"/>
+      <rgbColor rgb="FF7F7F7F"/>
+      <rgbColor rgb="FFEEEEEE"/>
+      <rgbColor rgb="FF9D44B8"/>
+      <rgbColor rgb="FFFFA93A"/>
+      <rgbColor rgb="FF63B2DE"/>
       <rgbColor rgb="00000000"/>
-      <rgbColor rgb="ffafe489"/>
-      <rgbColor rgb="ffff2c21"/>
-      <rgbColor rgb="ff357ca2"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="FFAFE489"/>
+      <rgbColor rgb="FFFF2C21"/>
+      <rgbColor rgb="FF357CA2"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FF008F00"/>
+    </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -1049,7 +1120,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -1058,7 +1129,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -1067,7 +1138,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -1076,7 +1147,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="20000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1085,7 +1156,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1094,7 +1165,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1206,8 +1277,8 @@
     <a:spDef>
       <a:spPr>
         <a:blipFill rotWithShape="1">
-          <a:blip r:embed="rId1"/>
-          <a:srcRect l="0" t="0" r="0" b="0"/>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:srcRect/>
           <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
         </a:blipFill>
         <a:ln w="12700" cap="flat">
@@ -1215,14 +1286,14 @@
           <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="50000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1241,7 +1312,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1249,7 +1320,7 @@
               <a:srgbClr val="FFFFFF"/>
             </a:solidFill>
             <a:effectLst>
-              <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="25400" dist="23998" dir="2700000">
+              <a:outerShdw blurRad="25400" dist="23998" dir="2700000" rotWithShape="0">
                 <a:srgbClr val="000000">
                   <a:alpha val="31034"/>
                 </a:srgbClr>
@@ -1277,7 +1348,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1303,7 +1374,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1329,7 +1400,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1355,7 +1426,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1381,7 +1452,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1407,7 +1478,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1433,7 +1504,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1459,7 +1530,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1485,7 +1556,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1498,9 +1569,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1516,7 +1593,7 @@
         </a:ln>
         <a:effectLst/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1535,7 +1612,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1561,7 +1638,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1587,7 +1664,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1613,7 +1690,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1639,7 +1716,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1665,7 +1742,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1691,7 +1768,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1717,7 +1794,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1743,7 +1820,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1769,7 +1846,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1782,9 +1859,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1797,7 +1880,7 @@
         </a:ln>
         <a:effectLst/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1816,7 +1899,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1846,7 +1929,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1872,7 +1955,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1898,7 +1981,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1924,7 +2007,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1950,7 +2033,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1976,7 +2059,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2002,7 +2085,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2028,7 +2111,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2054,7 +2137,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2067,548 +2150,555 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:IV31"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.125" style="1" customWidth="1"/>
+    <col min="1" max="7" width="9.125" style="1" customWidth="1"/>
     <col min="8" max="8" width="2.125" style="1" customWidth="1"/>
     <col min="9" max="9" width="25.125" style="1" customWidth="1"/>
     <col min="10" max="256" width="9" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="19" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="4"/>
-    </row>
-    <row r="2" ht="20.6" customHeight="1">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="7"/>
-    </row>
-    <row r="3" ht="20.6" customHeight="1">
-      <c r="A3" s="8">
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="70"/>
+    </row>
+    <row r="2" spans="1:9" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="1:9" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
         <v>12345</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="6">
         <v>12345</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="7">
         <v>12345</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="8">
         <v>12345</v>
       </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" t="s" s="13">
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" ht="20.25" customHeight="1">
-      <c r="A4" s="8">
-        <v>3.14159265</v>
-      </c>
-      <c r="B4" s="14">
-        <v>3.14159265</v>
-      </c>
-      <c r="C4" s="15">
-        <v>3.14159265</v>
-      </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-    </row>
-    <row r="5" ht="20.25" customHeight="1">
-      <c r="A5" s="16">
-        <v>3e-19</v>
-      </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-    </row>
-    <row r="6" ht="20.25" customHeight="1">
-      <c r="A6" s="17">
+    <row r="4" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>3.1415926500000002</v>
+      </c>
+      <c r="B4" s="11">
+        <v>3.1415926500000002</v>
+      </c>
+      <c r="C4" s="12">
+        <v>3.1415926500000002</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+    </row>
+    <row r="5" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="13">
+        <v>2.9999999999999999E-19</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="14">
         <v>41.33</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-    </row>
-    <row r="7" ht="20.25" customHeight="1">
-      <c r="A7" s="18">
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+    </row>
+    <row r="7" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="15">
         <v>34274</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-    </row>
-    <row r="8" ht="20.25" customHeight="1">
-      <c r="A8" s="19">
-        <v>0.06350694444444445</v>
-      </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-    </row>
-    <row r="9" ht="20.25" customHeight="1">
-      <c r="A9" s="20">
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="16">
+        <v>6.3506944444444449E-2</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+    </row>
+    <row r="9" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="17">
         <v>40841.258333333331</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-    </row>
-    <row r="10" ht="20.25" customHeight="1">
-      <c r="A10" s="20">
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="17">
         <v>40841.759027777778</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-    </row>
-    <row r="11" ht="20.25" customHeight="1">
-      <c r="A11" s="17">
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+    </row>
+    <row r="11" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="14">
         <v>-3.01</v>
       </c>
-      <c r="B11" s="21">
+      <c r="B11" s="18">
         <v>-3.01</v>
       </c>
-      <c r="C11" s="22">
+      <c r="C11" s="19">
         <v>-3.01</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-    </row>
-    <row r="12" ht="20.25" customHeight="1">
-      <c r="A12" s="8">
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
         <f>A3</f>
         <v>12345</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-    </row>
-    <row r="13" ht="20.25" customHeight="1">
-      <c r="A13" s="8">
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+    </row>
+    <row r="13" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
         <f>A3*2</f>
         <v>24690</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-    </row>
-    <row r="14" ht="20.25" customHeight="1">
-      <c r="A14" s="8">
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
         <v>123456789</v>
       </c>
-      <c r="B14" s="23">
+      <c r="B14" s="20">
         <v>12345679</v>
       </c>
-      <c r="C14" s="23">
+      <c r="C14" s="20">
         <v>12345679</v>
       </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-    </row>
-    <row r="15" ht="20.25" customHeight="1">
-      <c r="A15" s="24"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-    </row>
-    <row r="16" ht="20.25" customHeight="1">
-      <c r="A16" t="s" s="8">
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+    </row>
+    <row r="15" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="21"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+    </row>
+    <row r="16" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-    </row>
-    <row r="17" ht="20.25" customHeight="1">
-      <c r="A17" s="8">
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+    </row>
+    <row r="17" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="e">
         <f>A16*2</f>
-      </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-    </row>
-    <row r="18" ht="20.25" customHeight="1">
-      <c r="A18" s="8">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="e">
         <f>1/0</f>
-      </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-    </row>
-    <row r="19" ht="24.1" customHeight="1">
-      <c r="A19" s="17">
-        <f t="shared" si="4" ref="A19:D19">1000000</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+    </row>
+    <row r="19" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="14">
+        <f t="shared" ref="A19:D19" si="0">1000000</f>
         <v>1000000</v>
       </c>
-      <c r="B19" s="25">
-        <f t="shared" si="4"/>
+      <c r="B19" s="22">
+        <f t="shared" si="0"/>
         <v>1000000</v>
       </c>
-      <c r="C19" s="26">
-        <f t="shared" si="4"/>
+      <c r="C19" s="23">
+        <f t="shared" si="0"/>
         <v>1000000</v>
       </c>
-      <c r="D19" s="27">
-        <f t="shared" si="4"/>
+      <c r="D19" s="24">
+        <f t="shared" si="0"/>
         <v>1000000</v>
       </c>
-      <c r="E19" s="28"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-    </row>
-    <row r="20" ht="25.5" customHeight="1">
-      <c r="A20" t="s" s="8">
+      <c r="E19" s="25"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+    </row>
+    <row r="20" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B20" t="s" s="29">
+      <c r="B20" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C20" t="s" s="30">
+      <c r="C20" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="D20" t="s" s="31">
+      <c r="D20" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E20" t="s" s="32">
+      <c r="E20" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-    </row>
-    <row r="21" ht="21.6" customHeight="1">
-      <c r="A21" t="s" s="8">
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+    </row>
+    <row r="21" spans="1:9" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B21" t="s" s="33">
+      <c r="B21" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C21" t="s" s="34">
+      <c r="C21" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D21" t="s" s="35">
+      <c r="D21" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-    </row>
-    <row r="22" ht="20.25" customHeight="1">
-      <c r="A22" t="s" s="8">
+      <c r="E21" s="71" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+    </row>
+    <row r="22" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B22" t="s" s="36">
+      <c r="B22" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C22" t="s" s="36">
+      <c r="C22" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-    </row>
-    <row r="23" ht="20.25" customHeight="1">
-      <c r="A23" s="8">
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+    </row>
+    <row r="23" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="5">
         <v>0.99</v>
       </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-    </row>
-    <row r="24" ht="20.25" customHeight="1">
-      <c r="A24" s="8">
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+    </row>
+    <row r="24" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="5">
         <v>0.1</v>
       </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-    </row>
-    <row r="25" ht="20.25" customHeight="1">
-      <c r="A25" s="8">
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+    </row>
+    <row r="25" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="5">
         <v>-1</v>
       </c>
-      <c r="B25" s="13">
+      <c r="B25" s="10">
         <v>-1</v>
       </c>
-      <c r="C25" s="13">
+      <c r="C25" s="10">
         <v>-1</v>
       </c>
-      <c r="D25" s="13">
+      <c r="D25" s="10">
         <v>-1</v>
       </c>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-    </row>
-    <row r="26" ht="20.25" customHeight="1">
-      <c r="A26" t="s" s="37">
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+    </row>
+    <row r="26" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B26" t="s" s="38">
+      <c r="B26" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C26" t="s" s="39">
+      <c r="C26" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="D26" t="s" s="40">
+      <c r="D26" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E26" t="s" s="36">
+      <c r="E26" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-    </row>
-    <row r="27" ht="61.95" customHeight="1">
-      <c r="A27" t="s" s="8">
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+    </row>
+    <row r="27" spans="1:9" ht="62" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B27" t="s" s="41">
+      <c r="B27" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C27" t="s" s="42">
+      <c r="C27" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="D27" t="s" s="43">
+      <c r="D27" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-    </row>
-    <row r="28" ht="32.25" customHeight="1">
-      <c r="A28" t="s" s="8">
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+    </row>
+    <row r="28" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B28" t="s" s="36">
+      <c r="B28" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="C28" t="s" s="36">
+      <c r="C28" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="44"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-    </row>
-    <row r="29" ht="32.25" customHeight="1">
-      <c r="A29" t="s" s="8">
+      <c r="D28" s="41"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+    </row>
+    <row r="29" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B29" t="s" s="45">
+      <c r="B29" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="46"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
-    </row>
-    <row r="30" ht="21.25" customHeight="1">
-      <c r="A30" t="s" s="8">
+      <c r="C29" s="43"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+    </row>
+    <row r="30" spans="1:9" ht="21.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B30" t="s" s="48">
+      <c r="B30" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="C30" t="s" s="49">
+      <c r="C30" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="D30" t="s" s="50">
+      <c r="D30" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="E30" t="s" s="51">
+      <c r="E30" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="F30" t="s" s="52">
+      <c r="F30" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="G30" t="s" s="53">
+      <c r="G30" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-    </row>
-    <row r="31" ht="30.25" customHeight="1">
-      <c r="A31" t="s" s="8">
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+    </row>
+    <row r="31" spans="1:9" ht="30.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B31" t="s" s="54">
+      <c r="B31" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="C31" t="s" s="55">
+      <c r="C31" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="D31" t="s" s="56">
+      <c r="D31" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="E31" t="s" s="57">
+      <c r="E31" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="F31" t="s" s="58">
+      <c r="F31" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="G31" s="59"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
+      <c r="G31" s="56"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="A22:C22">
-    <cfRule type="containsText" dxfId="0" priority="1" stopIfTrue="1" text="conditional">
+    <cfRule type="containsText" dxfId="0" priority="1" stopIfTrue="1" operator="containsText" text="conditional">
       <formula>NOT(ISERROR(FIND(UPPER("conditional"),UPPER(A22))))</formula>
       <formula>"conditional"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
@@ -2616,97 +2706,93 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:IV10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="1" style="60" customWidth="1"/>
-    <col min="2" max="2" width="12.25" style="60" customWidth="1"/>
-    <col min="3" max="3" width="12.25" style="60" customWidth="1"/>
-    <col min="4" max="4" width="12.25" style="60" customWidth="1"/>
-    <col min="5" max="5" width="12.25" style="60" customWidth="1"/>
-    <col min="6" max="256" width="12.25" style="60" customWidth="1"/>
+    <col min="1" max="1" width="1" style="57" customWidth="1"/>
+    <col min="2" max="256" width="12.25" style="57" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="8" customHeight="1">
-      <c r="A1" s="61"/>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="63"/>
-    </row>
-    <row r="2" ht="20.55" customHeight="1">
-      <c r="A2" s="64"/>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-    </row>
-    <row r="3" ht="20.55" customHeight="1">
-      <c r="A3" s="64"/>
-      <c r="B3" s="66"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-    </row>
-    <row r="4" ht="20.35" customHeight="1">
-      <c r="A4" s="64"/>
-      <c r="B4" s="66"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-    </row>
-    <row r="5" ht="20.35" customHeight="1">
-      <c r="A5" s="64"/>
-      <c r="B5" s="66"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-    </row>
-    <row r="6" ht="20.35" customHeight="1">
-      <c r="A6" s="64"/>
-      <c r="B6" s="66"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-    </row>
-    <row r="7" ht="20.35" customHeight="1">
-      <c r="A7" s="64"/>
-      <c r="B7" s="66"/>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-    </row>
-    <row r="8" ht="20.35" customHeight="1">
-      <c r="A8" s="64"/>
-      <c r="B8" s="66"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-    </row>
-    <row r="9" ht="20.35" customHeight="1">
-      <c r="A9" s="64"/>
-      <c r="B9" s="66"/>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-    </row>
-    <row r="10" ht="20.35" customHeight="1">
-      <c r="A10" s="68"/>
-      <c r="B10" s="66"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
+    <row r="1" spans="1:5" ht="8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="58"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="60"/>
+    </row>
+    <row r="2" spans="1:5" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="61"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+    </row>
+    <row r="3" spans="1:5" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="61"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+    </row>
+    <row r="4" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="61"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+    </row>
+    <row r="5" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="61"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+    </row>
+    <row r="6" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="61"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+    </row>
+    <row r="7" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="61"/>
+      <c r="B7" s="63"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+    </row>
+    <row r="8" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="61"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+    </row>
+    <row r="9" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="61"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+    </row>
+    <row r="10" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="65"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="64"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
@@ -2714,97 +2800,93 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:IV10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="1" style="69" customWidth="1"/>
-    <col min="2" max="2" width="12.25" style="69" customWidth="1"/>
-    <col min="3" max="3" width="12.25" style="69" customWidth="1"/>
-    <col min="4" max="4" width="12.25" style="69" customWidth="1"/>
-    <col min="5" max="5" width="12.25" style="69" customWidth="1"/>
-    <col min="6" max="256" width="12.25" style="69" customWidth="1"/>
+    <col min="1" max="1" width="1" style="66" customWidth="1"/>
+    <col min="2" max="256" width="12.25" style="66" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="8" customHeight="1">
-      <c r="A1" s="61"/>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="63"/>
-    </row>
-    <row r="2" ht="20.55" customHeight="1">
-      <c r="A2" s="64"/>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-    </row>
-    <row r="3" ht="20.55" customHeight="1">
-      <c r="A3" s="64"/>
-      <c r="B3" s="66"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-    </row>
-    <row r="4" ht="20.35" customHeight="1">
-      <c r="A4" s="64"/>
-      <c r="B4" s="66"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-    </row>
-    <row r="5" ht="20.35" customHeight="1">
-      <c r="A5" s="64"/>
-      <c r="B5" s="66"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-    </row>
-    <row r="6" ht="20.35" customHeight="1">
-      <c r="A6" s="64"/>
-      <c r="B6" s="66"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-    </row>
-    <row r="7" ht="20.35" customHeight="1">
-      <c r="A7" s="64"/>
-      <c r="B7" s="66"/>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-    </row>
-    <row r="8" ht="20.35" customHeight="1">
-      <c r="A8" s="64"/>
-      <c r="B8" s="66"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-    </row>
-    <row r="9" ht="20.35" customHeight="1">
-      <c r="A9" s="64"/>
-      <c r="B9" s="66"/>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-    </row>
-    <row r="10" ht="20.35" customHeight="1">
-      <c r="A10" s="68"/>
-      <c r="B10" s="66"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
+    <row r="1" spans="1:5" ht="8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="58"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="60"/>
+    </row>
+    <row r="2" spans="1:5" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="61"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+    </row>
+    <row r="3" spans="1:5" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="61"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+    </row>
+    <row r="4" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="61"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+    </row>
+    <row r="5" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="61"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+    </row>
+    <row r="6" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="61"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+    </row>
+    <row r="7" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="61"/>
+      <c r="B7" s="63"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+    </row>
+    <row r="8" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="61"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+    </row>
+    <row r="9" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="61"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+    </row>
+    <row r="10" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="65"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="64"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
@@ -2812,97 +2894,93 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:IV10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="1" style="70" customWidth="1"/>
-    <col min="2" max="2" width="12.25" style="70" customWidth="1"/>
-    <col min="3" max="3" width="12.25" style="70" customWidth="1"/>
-    <col min="4" max="4" width="12.25" style="70" customWidth="1"/>
-    <col min="5" max="5" width="12.25" style="70" customWidth="1"/>
-    <col min="6" max="256" width="12.25" style="70" customWidth="1"/>
+    <col min="1" max="1" width="1" style="67" customWidth="1"/>
+    <col min="2" max="256" width="12.25" style="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="8" customHeight="1">
-      <c r="A1" s="61"/>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="63"/>
-    </row>
-    <row r="2" ht="20.55" customHeight="1">
-      <c r="A2" s="64"/>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-    </row>
-    <row r="3" ht="20.55" customHeight="1">
-      <c r="A3" s="64"/>
-      <c r="B3" s="66"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-    </row>
-    <row r="4" ht="20.35" customHeight="1">
-      <c r="A4" s="64"/>
-      <c r="B4" s="66"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-    </row>
-    <row r="5" ht="20.35" customHeight="1">
-      <c r="A5" s="64"/>
-      <c r="B5" s="66"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-    </row>
-    <row r="6" ht="20.35" customHeight="1">
-      <c r="A6" s="64"/>
-      <c r="B6" s="66"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-    </row>
-    <row r="7" ht="20.35" customHeight="1">
-      <c r="A7" s="64"/>
-      <c r="B7" s="66"/>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-    </row>
-    <row r="8" ht="20.35" customHeight="1">
-      <c r="A8" s="64"/>
-      <c r="B8" s="66"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-    </row>
-    <row r="9" ht="20.35" customHeight="1">
-      <c r="A9" s="64"/>
-      <c r="B9" s="66"/>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-    </row>
-    <row r="10" ht="20.35" customHeight="1">
-      <c r="A10" s="68"/>
-      <c r="B10" s="66"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
+    <row r="1" spans="1:5" ht="8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="58"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="60"/>
+    </row>
+    <row r="2" spans="1:5" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="61"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+    </row>
+    <row r="3" spans="1:5" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="61"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+    </row>
+    <row r="4" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="61"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+    </row>
+    <row r="5" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="61"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+    </row>
+    <row r="6" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="61"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+    </row>
+    <row r="7" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="61"/>
+      <c r="B7" s="63"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+    </row>
+    <row r="8" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="61"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+    </row>
+    <row r="9" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="61"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+    </row>
+    <row r="10" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="65"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="64"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>

</xml_diff>